<commit_message>
1.added ProductDetials class to get the price of the product in the product specific page 2.Modified the data sheet too.
</commit_message>
<xml_diff>
--- a/flipkartTesting/flip_data.xlsx
+++ b/flipkartTesting/flip_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13830" windowHeight="2520"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="14070" windowHeight="2535"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -79,7 +79,7 @@
     <t>Literature &amp; Fiction</t>
   </si>
   <si>
-    <t>Shri Ramcharitmanas</t>
+    <t>Shrimad Bhagvadgita</t>
   </si>
 </sst>
 </file>
@@ -451,7 +451,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>